<commit_message>
[ƒix] corrected some errors in the catalog
</commit_message>
<xml_diff>
--- a/CatalogoEstructurado.xlsx
+++ b/CatalogoEstructurado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egi/work/VirtualEnvs/AI/procesado_pedidos/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egi/work/VirtualEnvs/AI/procesado_pedidos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924FC34B-A6DA-0940-BF88-23EBB4DCA0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541F033-BAB9-0C46-BE64-919C7AD997B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10780" yWindow="-26980" windowWidth="35220" windowHeight="22600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24800" yWindow="-26700" windowWidth="35220" windowHeight="22600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructurado" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="199">
   <si>
     <t>583</t>
   </si>
@@ -577,30 +577,12 @@
     <t>QUESO MEZCLA PASTEURIZADO SEMICURADO</t>
   </si>
   <si>
-    <t>QUESO OVEJA LECHE CRUDA GRAN RESERVA</t>
-  </si>
-  <si>
     <t>QUESO OVEJA LECHE CRUDA AHUMADO</t>
   </si>
   <si>
-    <t>QUESO OVEJA LECHE CRUDA VP</t>
-  </si>
-  <si>
-    <t>QUESO OVEJA LECHE CRUDA ARTESANO</t>
-  </si>
-  <si>
-    <t>LECHE CRUDA ARTESANO</t>
-  </si>
-  <si>
     <t>VIRUTAS DE JAMON</t>
   </si>
   <si>
-    <t>PALETA DE BELLOTA IBERICA LONCHEADA</t>
-  </si>
-  <si>
-    <t>PANCETA DE BELLOTA IBERICA EMBUCHADA LONCHEADA</t>
-  </si>
-  <si>
     <t>PESO</t>
   </si>
   <si>
@@ -635,6 +617,18 @@
   </si>
   <si>
     <t>LONCHEADO LOMO</t>
+  </si>
+  <si>
+    <t>LONCEHADO 100 GR PALETA DE BELLOTA IBERICA</t>
+  </si>
+  <si>
+    <t>QUESO OVEJA LECHE CRUDA GRAN RESERVA 750 G</t>
+  </si>
+  <si>
+    <t>QUESO OVEJA LECHE CRUDA GRAN RESERVA 400 G</t>
+  </si>
+  <si>
+    <t>LONCEHADO 100 GR PANCETA DE BELLOTA IBERICA EMBUCHADA</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1218,13 +1212,13 @@
         <v>104</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>176</v>
@@ -1951,7 +1945,7 @@
         <v>120</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E34" s="3">
         <v>500</v>
@@ -2176,7 +2170,7 @@
         <v>75</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>118</v>
@@ -2196,7 +2190,7 @@
         <v>5341</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>103</v>
@@ -2204,7 +2198,7 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="1"/>
@@ -2220,7 +2214,7 @@
         <v>77</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>107</v>
@@ -2236,17 +2230,17 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="6">
-        <v>5461</v>
+      <c r="A47" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>187</v>
+        <v>79</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E47" s="3">
         <v>100</v>
@@ -2255,21 +2249,21 @@
       <c r="G47" s="3"/>
       <c r="H47" s="1"/>
       <c r="J47" s="5">
-        <v>11.95</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E48" s="3">
         <v>100</v>
@@ -2278,21 +2272,21 @@
       <c r="G48" s="3"/>
       <c r="H48" s="1"/>
       <c r="J48" s="5">
-        <v>4.5</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
-        <v>80</v>
+      <c r="A49" s="6">
+        <v>54611</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>81</v>
+        <v>195</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E49" s="3">
         <v>100</v>
@@ -2301,7 +2295,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="1"/>
       <c r="J49" s="5">
-        <v>3.95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2309,10 +2303,10 @@
         <v>54612</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>118</v>
@@ -2335,7 +2329,7 @@
         <v>83</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>118</v>
@@ -2503,7 +2497,7 @@
         <v>4253</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>141</v>
@@ -2512,7 +2506,7 @@
         <v>146</v>
       </c>
       <c r="E58" s="3">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2526,7 +2520,7 @@
         <v>4254</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>141</v>
@@ -2546,68 +2540,74 @@
     </row>
     <row r="60" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6">
-        <v>4256</v>
+        <v>4255</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E60" s="3">
         <v>750</v>
       </c>
       <c r="F60" s="3"/>
-      <c r="G60" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="G60" s="3"/>
       <c r="H60" s="1"/>
-      <c r="J60" s="5"/>
+      <c r="J60" s="5">
+        <v>15.85</v>
+      </c>
     </row>
     <row r="61" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="6">
-        <v>4257</v>
+      <c r="A61" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>184</v>
+        <v>93</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="E61" s="3">
-        <v>750</v>
-      </c>
-      <c r="F61" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G61" s="3"/>
       <c r="H61" s="1"/>
-      <c r="J61" s="5"/>
+      <c r="J61" s="5">
+        <v>5.95</v>
+      </c>
     </row>
     <row r="62" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E62" s="3">
         <v>500</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G62" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="H62" s="1"/>
       <c r="J62" s="5">
         <v>5.95</v>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="63" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>155</v>
@@ -2630,10 +2630,10 @@
         <v>500</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H63" s="1"/>
       <c r="J63" s="5">
@@ -2642,10 +2642,10 @@
     </row>
     <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>155</v>
@@ -2657,10 +2657,10 @@
         <v>500</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H64" s="1"/>
       <c r="J64" s="5">
@@ -2669,57 +2669,30 @@
     </row>
     <row r="65" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E65" s="3">
         <v>500</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>194</v>
-      </c>
+      <c r="F65" s="3"/>
       <c r="G65" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H65" s="1"/>
       <c r="J65" s="5">
-        <v>5.95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E66" s="3">
-        <v>500</v>
-      </c>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H66" s="1"/>
-      <c r="J66" s="5">
         <v>3.95</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[fix] missed element 5462
</commit_message>
<xml_diff>
--- a/CatalogoEstructurado.xlsx
+++ b/CatalogoEstructurado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egi/work/VirtualEnvs/AI/procesado_pedidos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541F033-BAB9-0C46-BE64-919C7AD997B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CAB36B-4D9D-9B44-B232-91665126330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="-26700" windowWidth="35220" windowHeight="22600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8000" yWindow="-24900" windowWidth="35220" windowHeight="23800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructurado" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="200">
   <si>
     <t>583</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>LONCEHADO 100 GR PANCETA DE BELLOTA IBERICA EMBUCHADA</t>
+  </si>
+  <si>
+    <t>LONCEHADO 100 GR JAMON DE BELLOTA IBERICO</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2230,17 +2233,17 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
-        <v>78</v>
+      <c r="A47" s="2">
+        <v>5462</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E47" s="3">
         <v>100</v>
@@ -2249,21 +2252,21 @@
       <c r="G47" s="3"/>
       <c r="H47" s="1"/>
       <c r="J47" s="5">
-        <v>4.5</v>
+        <v>11.95</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E48" s="3">
         <v>100</v>
@@ -2272,21 +2275,21 @@
       <c r="G48" s="3"/>
       <c r="H48" s="1"/>
       <c r="J48" s="5">
-        <v>3.95</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="6">
-        <v>54611</v>
+      <c r="A49" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>195</v>
+        <v>81</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>191</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E49" s="3">
         <v>100</v>
@@ -2295,18 +2298,18 @@
       <c r="G49" s="3"/>
       <c r="H49" s="1"/>
       <c r="J49" s="5">
-        <v>5</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6">
-        <v>54612</v>
+        <v>54611</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>118</v>
@@ -2318,18 +2321,18 @@
       <c r="G50" s="3"/>
       <c r="H50" s="1"/>
       <c r="J50" s="5">
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
-        <v>82</v>
+      <c r="A51" s="6">
+        <v>54612</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>83</v>
+        <v>198</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>118</v>
@@ -2346,85 +2349,83 @@
     </row>
     <row r="52" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="E52" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>138</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="1"/>
       <c r="J52" s="5">
-        <v>13</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E53" s="3">
-        <v>2000</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3" t="s">
-        <v>140</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="3"/>
       <c r="H53" s="1"/>
       <c r="J53" s="5">
-        <v>12.2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E54" s="3">
-        <v>750</v>
+        <v>2000</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H54" s="1"/>
       <c r="J54" s="5">
-        <v>13.5</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>141</v>
@@ -2437,19 +2438,19 @@
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H55" s="1"/>
       <c r="J55" s="5">
-        <v>15.35</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="6">
-        <v>4251</v>
+      <c r="A56" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>141</v>
@@ -2462,94 +2463,96 @@
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="H56" s="1"/>
       <c r="J56" s="5">
-        <v>8.6999999999999993</v>
+        <v>15.35</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6">
-        <v>4252</v>
+        <v>4251</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E57" s="3">
         <v>750</v>
       </c>
       <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="H57" s="1"/>
       <c r="J57" s="5">
-        <v>4.6500000000000004</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6">
-        <v>4253</v>
+        <v>4252</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E58" s="3">
-        <v>400</v>
+        <v>750</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="1"/>
       <c r="J58" s="5">
-        <v>8.15</v>
+        <v>4.6500000000000004</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6">
-        <v>4254</v>
+        <v>4253</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E59" s="3">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="1"/>
       <c r="J59" s="5">
-        <v>8.5</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6">
-        <v>4255</v>
+        <v>4254</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E60" s="3">
         <v>750</v>
@@ -2558,46 +2561,44 @@
       <c r="G60" s="3"/>
       <c r="H60" s="1"/>
       <c r="J60" s="5">
-        <v>15.85</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
-        <v>92</v>
+      <c r="A61" s="6">
+        <v>4255</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>93</v>
+        <v>196</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E61" s="3">
-        <v>500</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>188</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="1"/>
       <c r="J61" s="5">
-        <v>5.95</v>
+        <v>15.85</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E62" s="3">
         <v>500</v>
@@ -2605,9 +2606,7 @@
       <c r="F62" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>158</v>
-      </c>
+      <c r="G62" s="3"/>
       <c r="H62" s="1"/>
       <c r="J62" s="5">
         <v>5.95</v>
@@ -2615,10 +2614,10 @@
     </row>
     <row r="63" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>155</v>
@@ -2633,7 +2632,7 @@
         <v>188</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H63" s="1"/>
       <c r="J63" s="5">
@@ -2642,10 +2641,10 @@
     </row>
     <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>155</v>
@@ -2660,7 +2659,7 @@
         <v>188</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H64" s="1"/>
       <c r="J64" s="5">
@@ -2669,30 +2668,57 @@
     </row>
     <row r="65" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E65" s="3">
         <v>500</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G65" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H65" s="1"/>
       <c r="J65" s="5">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" s="3">
+        <v>500</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H66" s="1"/>
+      <c r="J66" s="5">
         <v>3.95</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>